<commit_message>
new tc on 185
</commit_message>
<xml_diff>
--- a/RBCC_E/configs/icf185.xlsx
+++ b/RBCC_E/configs/icf185.xlsx
@@ -15356,7 +15356,7 @@
   <dimension ref="A1:CG55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="BV1" workbookViewId="0">
-      <selection activeCell="BW12" sqref="BW12"/>
+      <selection activeCell="CG13" sqref="CG13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18513,37 +18513,37 @@
         <v>1565</v>
       </c>
       <c r="BW12" s="20">
-        <v>1565</v>
+        <v>1540</v>
       </c>
       <c r="BX12" s="20">
-        <v>1565</v>
+        <v>1540</v>
       </c>
       <c r="BY12" s="20">
-        <v>1565</v>
+        <v>1540</v>
       </c>
       <c r="BZ12" s="20">
-        <v>1565</v>
+        <v>1540</v>
       </c>
       <c r="CA12" s="20">
-        <v>1565</v>
+        <v>1540</v>
       </c>
       <c r="CB12" s="20">
-        <v>1565</v>
+        <v>1540</v>
       </c>
       <c r="CC12" s="20">
-        <v>1565</v>
+        <v>1540</v>
       </c>
       <c r="CD12" s="20">
-        <v>1565</v>
+        <v>1540</v>
       </c>
       <c r="CE12" s="20">
-        <v>1565</v>
+        <v>1540</v>
       </c>
       <c r="CF12" s="20">
-        <v>1565</v>
+        <v>1540</v>
       </c>
       <c r="CG12" s="20">
-        <v>1565</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="13" spans="1:85" x14ac:dyDescent="0.2">

</xml_diff>